<commit_message>
changed the link property
</commit_message>
<xml_diff>
--- a/design_docs/TranslationAutomation/design_for_automl_feeder.xlsx
+++ b/design_docs/TranslationAutomation/design_for_automl_feeder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWu\alexwusdoc_cnt\alexwusdoc\automl_feeder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWu\jcc_doc_cnt\documentation\design_docs\TranslationAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA87210-7D34-41E7-988C-B4845D1B81C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580612F-D26D-4BCC-90D7-65ECDF91506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{2700FEFF-BC8D-4CF4-8093-E5B99C7F40C3}"/>
   </bookViews>
@@ -103,12 +103,6 @@
     <t>End Loop</t>
   </si>
   <si>
-    <t>Drawing 2.vsdx (sharepoint.com)</t>
-  </si>
-  <si>
-    <t>Drawing1.vsdx (sharepoint.com)</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -410,6 +404,12 @@
   </si>
   <si>
     <t>not an issue</t>
+  </si>
+  <si>
+    <t>user_case_view.vsdx (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>entity_view.vsdx (sharepoint.com)</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1072,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,16 +1085,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
         <v>82</v>
-      </c>
-      <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1148,10 +1148,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -1176,11 +1176,11 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1216,56 +1216,56 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1278,9 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D66A41A6-8648-4BE0-96D5-EC9BBCB6A85E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1291,12 +1289,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>20</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://caljc-my.sharepoint.com/:u:/r/personal/alex_wu_jud_ca_gov/_layouts/15/Doc.aspx?sourcedoc=%7B70855C5D-2233-4F70-B7CE-D2C86C0A5306%7D&amp;file=Drawing%202.vsdx&amp;action=edit&amp;mobileredirect=true&amp;wdnewandopenct=0&amp;ct=1716871072295&amp;wdOrigin=OFFICECOM-HWA.START.NEW&amp;wdPreviousSessionSrc=HarmonyDesktop&amp;wdPreviousSession=c934dee2-ea14-4a3a-a488-ea7db4d3f786&amp;cid=ef2b0e3c-f1e6-4855-859c-c7ea896b1fad&amp;or=PrevCreateNew" xr:uid="{B8BC65A7-2091-407F-89B1-5CC14BB36D0E}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{B8BC65A7-2091-407F-89B1-5CC14BB36D0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1308,19 +1306,19 @@
   <dimension ref="B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X20" sqref="X20"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>21</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://caljc-my.sharepoint.com/:u:/r/personal/alex_wu_jud_ca_gov/_layouts/15/Doc.aspx?sourcedoc=%7B4d6fc3fb-78ce-49b5-9e0e-70c1f76300f6%7D&amp;action=edit&amp;wdPreviousSession=c69ccdeb-e07d-4fc8-58bb-7243f2cbd1c1&amp;wdnewandopenct=0&amp;wdo=4&amp;wdOrigin=wacFileNew&amp;wdTpl=blank&amp;wdLcid=1033&amp;wdPreviousCorrelation=0e1a3f28-2fdc-4132-adb1-5a0de5812d4f&amp;or=PrevCreateNew" xr:uid="{D33CC299-0AC9-48FE-B61C-16BF6EAE515E}"/>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{D33CC299-0AC9-48FE-B61C-16BF6EAE515E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
@@ -1344,352 +1342,352 @@
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D3" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D14" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
         <v>27</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="23" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D34" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D39" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D43" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E47" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" t="s">
         <v>71</v>
-      </c>
-      <c r="E51" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E52" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E54" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D57" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E57" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E61" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D65" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1712,28 +1710,28 @@
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
         <v>100</v>
-      </c>
-      <c r="E3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further improvement to the design, making the points more clear
</commit_message>
<xml_diff>
--- a/design_docs/TranslationAutomation/design_for_automl_feeder.xlsx
+++ b/design_docs/TranslationAutomation/design_for_automl_feeder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWu\jcc_doc_cnt\documentation\design_docs\TranslationAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2580612F-D26D-4BCC-90D7-65ECDF91506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8270A14-12F9-45A8-9220-E5C995039D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{2700FEFF-BC8D-4CF4-8093-E5B99C7F40C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2700FEFF-BC8D-4CF4-8093-E5B99C7F40C3}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Highlevel View" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="128">
   <si>
     <t>VCSC Canned Responses</t>
   </si>
@@ -280,15 +280,9 @@
     <t>SME users, system operation users, and super users</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>Use</t>
   </si>
   <si>
@@ -410,6 +404,27 @@
   </si>
   <si>
     <t>entity_view.vsdx (sharepoint.com)</t>
+  </si>
+  <si>
+    <t>Goal</t>
+  </si>
+  <si>
+    <t>collect a pile of language pairs, and vaidate them, and upload them to AutoML</t>
+  </si>
+  <si>
+    <t>Essence</t>
+  </si>
+  <si>
+    <t>Extract</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Transfor</t>
+  </si>
+  <si>
+    <t>It's a ELT project!</t>
   </si>
 </sst>
 </file>
@@ -493,7 +508,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -581,6 +596,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -589,7 +619,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -601,9 +631,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1040,61 +1075,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCE64B5-9469-40BB-A811-E81488946791}">
-  <dimension ref="A5:E13"/>
+  <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" t="s">
         <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1148,10 +1225,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1163,7 +1240,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -1176,11 +1253,11 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1201,10 +1278,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1216,56 +1293,56 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1289,7 +1366,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1313,7 +1390,7 @@
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1342,7 +1419,7 @@
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
@@ -1379,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -1448,7 +1525,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
@@ -1515,17 +1592,17 @@
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
@@ -1535,15 +1612,15 @@
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D34" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E34" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
@@ -1656,30 +1733,30 @@
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E61" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.25">
@@ -1699,7 +1776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F71351-6733-4CB3-A9FB-37AD2538CB96}">
   <dimension ref="C2:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1710,28 +1787,28 @@
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" t="s">
         <v>98</v>
-      </c>
-      <c r="E3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some improvement, based on the inputs from audience on 5/31
</commit_message>
<xml_diff>
--- a/design_docs/TranslationAutomation/design_for_automl_feeder.xlsx
+++ b/design_docs/TranslationAutomation/design_for_automl_feeder.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWu\jcc_doc_cnt\documentation\design_docs\TranslationAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AWu\jcc_doc_cnt_new\documentation\design_docs\TranslationAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8270A14-12F9-45A8-9220-E5C995039D3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC343E36-93FD-4A63-83C8-758B81547596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2700FEFF-BC8D-4CF4-8093-E5B99C7F40C3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{2700FEFF-BC8D-4CF4-8093-E5B99C7F40C3}"/>
   </bookViews>
   <sheets>
     <sheet name="1_Highlevel View" sheetId="3" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="132">
   <si>
     <t>VCSC Canned Responses</t>
   </si>
@@ -250,15 +250,9 @@
     <t>unreviewed</t>
   </si>
   <si>
-    <t>signoffed</t>
-  </si>
-  <si>
     <t>uploaded to AutoML, happens only after sign-ed off</t>
   </si>
   <si>
-    <t>by project or product managers, only after validated</t>
-  </si>
-  <si>
     <t>invalid</t>
   </si>
   <si>
@@ -331,9 +325,6 @@
     <t>security</t>
   </si>
   <si>
-    <t>watermarking sensitive ingested data</t>
-  </si>
-  <si>
     <t>PHI</t>
   </si>
   <si>
@@ -421,17 +412,38 @@
     <t>Load</t>
   </si>
   <si>
-    <t>Transfor</t>
-  </si>
-  <si>
     <t>It's a ELT project!</t>
+  </si>
+  <si>
+    <t>Transform</t>
+  </si>
+  <si>
+    <t>######1234</t>
+  </si>
+  <si>
+    <t>column level security</t>
+  </si>
+  <si>
+    <t>row level security</t>
+  </si>
+  <si>
+    <t>rdbms</t>
+  </si>
+  <si>
+    <t>masking sensitive ingested data</t>
+  </si>
+  <si>
+    <t>can we do that in cosmosdb?</t>
+  </si>
+  <si>
+    <t>custom logic to filter off those sensitive data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +492,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -633,12 +653,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1077,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCE64B5-9469-40BB-A811-E81488946791}">
   <dimension ref="B2:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,18 +1112,18 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
         <v>123</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1117,28 +1137,22 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="13"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="17" t="s">
-        <v>81</v>
+      <c r="E9" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -1146,15 +1160,12 @@
       <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1162,16 +1173,16 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" t="s">
         <v>124</v>
       </c>
-      <c r="D14" t="s">
-        <v>125</v>
-      </c>
-      <c r="E14" t="s">
-        <v>126</v>
-      </c>
       <c r="F14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1184,7 +1195,7 @@
   <dimension ref="B4:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,10 +1236,10 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1240,7 +1251,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -1253,11 +1264,11 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1278,10 +1289,10 @@
         <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1293,56 +1304,56 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1366,7 +1377,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1382,15 +1393,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C304ADD6-94CA-4EBB-A7E7-78285E267EA8}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1406,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{456C77BA-D336-4735-AE8F-44E7E8CD8672}">
   <dimension ref="C2:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,7 +1430,7 @@
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
@@ -1456,7 +1467,7 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -1525,7 +1536,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
@@ -1567,17 +1578,17 @@
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
@@ -1592,35 +1603,35 @@
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D34" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
@@ -1694,28 +1705,20 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>69</v>
-      </c>
-      <c r="E51" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>37</v>
       </c>
       <c r="E52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.25">
@@ -1733,30 +1736,30 @@
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E61" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.25">
@@ -1764,7 +1767,7 @@
         <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1774,10 +1777,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47F71351-6733-4CB3-A9FB-37AD2538CB96}">
-  <dimension ref="C2:F10"/>
+  <dimension ref="C2:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,30 +1788,70 @@
     <col min="4" max="4" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D4" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D5" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>